<commit_message>
Exporting EXCEL sheets + fixed pos back button
</commit_message>
<xml_diff>
--- a/inventory_reports.xlsx
+++ b/inventory_reports.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="83">
   <si>
     <t>Product_ID</t>
   </si>
@@ -111,6 +111,9 @@
     <t>PRD015</t>
   </si>
   <si>
+    <t>PRD016</t>
+  </si>
+  <si>
     <t>Coca-Cola (330ml)</t>
   </si>
   <si>
@@ -156,6 +159,9 @@
     <t>Mountain Dew (350ml)</t>
   </si>
   <si>
+    <t>Nestea (330ml)</t>
+  </si>
+  <si>
     <t>2024-11-25</t>
   </si>
   <si>
@@ -201,6 +207,9 @@
     <t>2024-12-05</t>
   </si>
   <si>
+    <t>2025-03-01</t>
+  </si>
+  <si>
     <t>In Stock</t>
   </si>
   <si>
@@ -234,7 +243,7 @@
     <t>09222345678</t>
   </si>
   <si>
-    <t>09171234567</t>
+    <t>09456123481</t>
   </si>
   <si>
     <t>09356789101</t>
@@ -243,7 +252,7 @@
     <t>orders@gourmetgrocers.com</t>
   </si>
   <si>
-    <t>info@freshfoods.com</t>
+    <t>info@tiamzonfoodco.com</t>
   </si>
   <si>
     <t>info@globalfooddist.com</t>
@@ -252,7 +261,7 @@
     <t>1356 Gen. Luna Street, Intramuros, Manila</t>
   </si>
   <si>
-    <t>1234 Mabini Street, Ermita, Manila</t>
+    <t>273 Harvard Avenue, Pasig</t>
   </si>
   <si>
     <t>345 P. Burgos Street, Makati</t>
@@ -680,7 +689,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -744,25 +753,25 @@
         <v>45463</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J2">
         <v>50</v>
@@ -771,19 +780,19 @@
         <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -794,25 +803,25 @@
         <v>45463</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3">
+        <v>59</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
         <v>64</v>
       </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>61</v>
-      </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J3">
         <v>100</v>
@@ -821,19 +830,19 @@
         <v>50</v>
       </c>
       <c r="L3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -844,25 +853,25 @@
         <v>45463</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J4">
         <v>100</v>
@@ -871,19 +880,19 @@
         <v>50</v>
       </c>
       <c r="L4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -894,7 +903,7 @@
         <v>45463</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>32</v>
@@ -903,16 +912,16 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J5">
         <v>120</v>
@@ -921,19 +930,19 @@
         <v>50</v>
       </c>
       <c r="L5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -944,7 +953,7 @@
         <v>45463</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -953,31 +962,31 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -988,7 +997,7 @@
         <v>45464</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -997,31 +1006,31 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1032,7 +1041,7 @@
         <v>45464</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -1041,31 +1050,31 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1076,7 +1085,7 @@
         <v>45464</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -1085,31 +1094,31 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1120,7 +1129,7 @@
         <v>45464</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>50</v>
@@ -1129,31 +1138,31 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1164,25 +1173,25 @@
         <v>45464</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J11">
         <v>55</v>
@@ -1191,19 +1200,19 @@
         <v>35</v>
       </c>
       <c r="L11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1214,7 +1223,7 @@
         <v>45465</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -1223,16 +1232,16 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J12">
         <v>60</v>
@@ -1241,19 +1250,19 @@
         <v>35</v>
       </c>
       <c r="L12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P12" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1264,7 +1273,7 @@
         <v>45465</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1273,16 +1282,16 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J13">
         <v>200</v>
@@ -1291,19 +1300,19 @@
         <v>90</v>
       </c>
       <c r="L13" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O13" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1314,7 +1323,7 @@
         <v>45465</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14">
         <v>39</v>
@@ -1323,16 +1332,16 @@
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J14">
         <v>180</v>
@@ -1341,19 +1350,19 @@
         <v>150</v>
       </c>
       <c r="L14" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1364,7 +1373,7 @@
         <v>45465</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1373,16 +1382,16 @@
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J15">
         <v>95</v>
@@ -1391,19 +1400,19 @@
         <v>50</v>
       </c>
       <c r="L15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N15" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O15" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1414,25 +1423,25 @@
         <v>45465</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E16">
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I16" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J16">
         <v>50</v>
@@ -1441,19 +1450,69 @@
         <v>35</v>
       </c>
       <c r="L16" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="M16" t="s">
+        <v>76</v>
+      </c>
+      <c r="N16" t="s">
+        <v>79</v>
+      </c>
+      <c r="O16" t="s">
+        <v>82</v>
+      </c>
+      <c r="P16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45465</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17">
+        <v>65</v>
+      </c>
+      <c r="K17">
+        <v>40</v>
+      </c>
+      <c r="L17" t="s">
         <v>73</v>
       </c>
-      <c r="N16" t="s">
+      <c r="M17" t="s">
         <v>76</v>
       </c>
-      <c r="O16" t="s">
+      <c r="N17" t="s">
         <v>79</v>
       </c>
-      <c r="P16" t="s">
-        <v>66</v>
+      <c r="O17" t="s">
+        <v>82</v>
+      </c>
+      <c r="P17" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1463,7 +1522,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1527,25 +1586,25 @@
         <v>45463</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J2">
         <v>50</v>
@@ -1554,19 +1613,19 @@
         <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1577,25 +1636,25 @@
         <v>45463</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3">
+        <v>59</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
         <v>64</v>
       </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>61</v>
-      </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J3">
         <v>100</v>
@@ -1604,19 +1663,19 @@
         <v>50</v>
       </c>
       <c r="L3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1627,25 +1686,25 @@
         <v>45463</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J4">
         <v>100</v>
@@ -1654,19 +1713,19 @@
         <v>50</v>
       </c>
       <c r="L4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1677,7 +1736,7 @@
         <v>45463</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>32</v>
@@ -1686,16 +1745,16 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J5">
         <v>120</v>
@@ -1704,19 +1763,19 @@
         <v>50</v>
       </c>
       <c r="L5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1727,7 +1786,7 @@
         <v>45463</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -1736,31 +1795,31 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1771,7 +1830,7 @@
         <v>45464</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -1780,31 +1839,31 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1815,7 +1874,7 @@
         <v>45464</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -1824,31 +1883,31 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1859,7 +1918,7 @@
         <v>45464</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -1868,31 +1927,31 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1903,7 +1962,7 @@
         <v>45464</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>50</v>
@@ -1912,31 +1971,31 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1947,25 +2006,25 @@
         <v>45464</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J11">
         <v>55</v>
@@ -1974,19 +2033,19 @@
         <v>35</v>
       </c>
       <c r="L11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1997,7 +2056,7 @@
         <v>45465</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -2006,16 +2065,16 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J12">
         <v>60</v>
@@ -2024,19 +2083,19 @@
         <v>35</v>
       </c>
       <c r="L12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P12" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2047,7 +2106,7 @@
         <v>45465</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2056,16 +2115,16 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J13">
         <v>200</v>
@@ -2074,19 +2133,19 @@
         <v>90</v>
       </c>
       <c r="L13" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O13" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2097,7 +2156,7 @@
         <v>45465</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14">
         <v>39</v>
@@ -2106,16 +2165,16 @@
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J14">
         <v>180</v>
@@ -2124,19 +2183,19 @@
         <v>150</v>
       </c>
       <c r="L14" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2147,7 +2206,7 @@
         <v>45465</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2156,16 +2215,16 @@
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J15">
         <v>95</v>
@@ -2174,19 +2233,19 @@
         <v>50</v>
       </c>
       <c r="L15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N15" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O15" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -2197,25 +2256,25 @@
         <v>45465</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E16">
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I16" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J16">
         <v>50</v>
@@ -2224,19 +2283,69 @@
         <v>35</v>
       </c>
       <c r="L16" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="M16" t="s">
+        <v>76</v>
+      </c>
+      <c r="N16" t="s">
+        <v>79</v>
+      </c>
+      <c r="O16" t="s">
+        <v>82</v>
+      </c>
+      <c r="P16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45465</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17">
+        <v>65</v>
+      </c>
+      <c r="K17">
+        <v>40</v>
+      </c>
+      <c r="L17" t="s">
         <v>73</v>
       </c>
-      <c r="N16" t="s">
+      <c r="M17" t="s">
         <v>76</v>
       </c>
-      <c r="O16" t="s">
+      <c r="N17" t="s">
         <v>79</v>
       </c>
-      <c r="P16" t="s">
-        <v>66</v>
+      <c r="O17" t="s">
+        <v>82</v>
+      </c>
+      <c r="P17" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>